<commit_message>
Added tests to the previously added methods
</commit_message>
<xml_diff>
--- a/JlgCommonTests/ExcelManager/ExcelReaderTestsFile.xlsx
+++ b/JlgCommonTests/ExcelManager/ExcelReaderTestsFile.xlsx
@@ -9,19 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Page1" sheetId="1" r:id="rId1"/>
     <sheet name="Page2" sheetId="2" r:id="rId2"/>
     <sheet name="Page3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
   <si>
     <t/>
   </si>
@@ -50,20 +50,17 @@
     <t>tests</t>
   </si>
   <si>
-    <t>H1</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>H3</t>
+    <t>Merged cells</t>
+  </si>
+  <si>
+    <t>searchedString</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -73,16 +70,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.24994659260841701"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -97,15 +106,95 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -121,18 +210,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C3" totalsRowShown="0">
-  <autoFilter ref="A1:C3"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="H1"/>
-    <tableColumn id="2" name="H2"/>
-    <tableColumn id="3" name="H3"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -400,7 +477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -542,55 +619,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>22</v>
-      </c>
-      <c r="C3">
-        <v>33</v>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>